<commit_message>
Enhance import/export functionality in Talinda POS system. Updated the Import/Export Guide to reflect new features, including product and category import/export options, template downloads, and improved error handling. Implemented backend methods for exporting and importing products and categories to/from Excel files, with options for updating existing items. Added UI components for import/export operations, including progress tracking and status updates.
</commit_message>
<xml_diff>
--- a/products_export_20250730_041449.xlsx
+++ b/products_export_20250730_041449.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5844"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -36,7 +36,7 @@
     <t>Barcode</t>
   </si>
   <si>
-    <t>Image_Path</t>
+    <t>Image Path</t>
   </si>
   <si>
     <t>الأطباق الرئيسية</t>
@@ -496,7 +496,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,26 +507,25 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1976D2"/>
+        <bgColor rgb="FF1976D2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -534,32 +533,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,11 +846,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -881,7 +869,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">

</xml_diff>